<commit_message>
Undo, mo phong van co, newgame
</commit_message>
<xml_diff>
--- a/bảng kế hoạch.xlsx
+++ b/bảng kế hoạch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\doan1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studying\Năm 3\Đồ án 1\doan1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B6EFA3-C8A4-4D17-92FA-AAEEA4C970D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E6D910-338C-4C04-8923-00C1AC0C3877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>STT</t>
   </si>
@@ -159,12 +159,19 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -314,7 +321,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -336,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -351,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,16 +367,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -396,13 +403,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -413,6 +420,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,22 +713,22 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="64.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25">
+    <row r="1" spans="1:10" ht="25.8">
       <c r="A1" s="27" t="s">
         <v>41</v>
       </c>
@@ -990,7 +1003,9 @@
       <c r="H11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="13"/>
+      <c r="I11" s="33">
+        <v>43740</v>
+      </c>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10">
@@ -1015,7 +1030,9 @@
       <c r="G12" s="20">
         <v>43756</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="34" t="s">
+        <v>35</v>
+      </c>
       <c r="I12" s="13"/>
       <c r="J12" s="4"/>
     </row>
@@ -1061,8 +1078,12 @@
       <c r="G14" s="20">
         <v>43758</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
+      <c r="H14" s="33">
+        <v>43740</v>
+      </c>
+      <c r="I14" s="33">
+        <v>43742</v>
+      </c>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10">
@@ -1085,8 +1106,12 @@
       <c r="G15" s="20">
         <v>43760</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="H15" s="33">
+        <v>43740</v>
+      </c>
+      <c r="I15" s="33">
+        <v>43742</v>
+      </c>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10">

</xml_diff>

<commit_message>
UPDATE hien quan co qua LAN
</commit_message>
<xml_diff>
--- a/bảng kế hoạch.xlsx
+++ b/bảng kế hoạch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studying\Năm 3\Đồ án 1\doan1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7540240C-5681-4777-8E30-ACAD25BFF520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5DC0C8-2513-473B-8858-601722F6D7A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -712,7 +712,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1053,8 +1053,12 @@
       <c r="G13" s="20">
         <v>43757</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
+      <c r="H13" s="22">
+        <v>43749</v>
+      </c>
+      <c r="I13" s="22">
+        <v>43757</v>
+      </c>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10">

</xml_diff>